<commit_message>
1.l upload wrappers integration alpha alg
</commit_message>
<xml_diff>
--- a/imputegap/analysis/run_0/eeg-alcohol/report_eeg-alcohol.xlsx
+++ b/imputegap/analysis/run_0/eeg-alcohol/report_eeg-alcohol.xlsx
@@ -32,7 +32,7 @@
     <t>Generated on</t>
   </si>
   <si>
-    <t>2025-01-22 16:56:05</t>
+    <t>2025-01-23 15:14:08</t>
   </si>
   <si>
     <t>Run Number</t>
@@ -59,7 +59,7 @@
     <t>eegalcohol</t>
   </si>
   <si>
-    <t>{'mcar': {'cdrec': {'bayesian': {'0.05': {'scores': {'RMSE': 0.2760534633653583, 'MAE': 0.20172179379755226, 'MI': 1.6287285825717355, 'CORRELATION': 0.9838005973658245}, 'times': {'contamination': 0.0010294914245605469, 'optimization': 6.223032236099243, 'imputation': 1.8180451393127441, 'log_imputation': 0.2596046618953402}}, '0.1': {'scores': {'RMSE': 0.23232694306396792, 'MAE': 0.17310574767639833, 'MI': 1.1951438022350207, 'CORRELATION': 0.9640385877101987}, 'times': {'contamination': 0.020868778228759766, 'optimization': 6.223032236099243, 'imputation': 2.9365129470825195, 'log_imputation': 0.4678319199871146}}, '0.2': {'scores': {'RMSE': 0.21804885816582126, 'MAE': 0.16264927399368442, 'MI': 1.184724280002774, 'CORRELATION': 0.9737339134318108}, 'times': {'contamination': 0.006024837493896484, 'optimization': 6.223032236099243, 'imputation': 7.126884460449219, 'log_imputation': 0.8528997181632954}}, '0.4': {'scores': {'RMSE': 0.2848440560052875, 'MAE': 0.1955094245129383, 'MI': 1.0150919512842373, 'CORRELATION': 0.9596099121939261}, 'times': {'contamination': 0.02350163459777832, 'optimization': 6.223032236099243, 'imputation': 17.258519649505615, 'log_imputation': 1.237003541343099}}, '0.6': {'scores': {'RMSE': 0.3411304383415171, 'MAE': 0.23465960462790822, 'MI': 0.8713081877855033, 'CORRELATION': 0.940224565771335}, 'times': {'contamination': 0.06571340560913086, 'optimization': 6.223032236099243, 'imputation': 35.12345743179321, 'log_imputation': 1.5455972597865577}}, '0.8': {'scores': {'RMSE': 0.5679458730957043, 'MAE': 0.3748930267443002, 'MI': 0.5716189408134524, 'CORRELATION': 0.8410496841608825}, 'times': {'contamination': 0.196336030960083, 'optimization': 6.223032236099243, 'imputation': 56.51965832710266, 'log_imputation': 1.7521995277854656}}}}, 'iter_svd': {'bayesian': {'0.05': {'scores': {'RMSE': 1.107394798606378, 'MAE': 0.9036474830477748, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0011682510375976562, 'optimization': 6.223032236099243, 'imputation': 0.0005362033843994141, 'log_imputation': -3.2706704491719543}}, '0.1': {'scores': {'RMSE': 0.8569349076796438, 'MAE': 0.6416542359734557, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00396728515625, 'optimization': 6.223032236099243, 'imputation': 0.0004646778106689453, 'log_imputation': -3.332848065489965}}, '0.2': {'scores': {'RMSE': 0.9609255264919324, 'MAE': 0.756013835497571, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0041027069091796875, 'optimization': 6.223032236099243, 'imputation': 0.0009090900421142578, 'log_imputation': -3.0413930993339156}}, '0.4': {'scores': {'RMSE': 1.0184989120725458, 'MAE': 0.8150966718352457, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.011993169784545898, 'optimization': 6.223032236099243, 'imputation': 0.0003638267517089844, 'log_imputation': -3.4391053709887247}}, '0.6': {'scores': {'RMSE': 0.9997401940199045, 'MAE': 0.7985721718600829, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.03504228591918945, 'optimization': 6.223032236099243, 'imputation': 0.0003619194030761719, 'log_imputation': -3.441388133048125}}, '0.8': {'scores': {'RMSE': 0.9895691678332014, 'MAE': 0.7901674118013952, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.17596697807312012, 'optimization': 6.223032236099243, 'imputation': 0.0005311965942382812, 'log_imputation': -3.274744718105895}}}}, 'grouse': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5148496955923699, 'MAE': 0.415876537807372, 'MI': 1.3401665927292032, 'CORRELATION': 0.9150576799948262}, 'times': {'contamination': 0.0004994869232177734, 'optimization': 6.223032236099243, 'imputation': 0.1745896339416504, 'log_imputation': -0.7579815455994404}}, '0.1': {'scores': {'RMSE': 0.5514172365414519, 'MAE': 0.4246206846745574, 'MI': 0.605160166686089, 'CORRELATION': 0.7646002717223995}, 'times': {'contamination': 0.0012345314025878906, 'optimization': 6.223032236099243, 'imputation': 0.04293513298034668, 'log_imputation': -1.3671871876495891}}, '0.2': {'scores': {'RMSE': 0.5224946657403522, 'MAE': 0.4039231091274249, 'MI': 0.6011853028388328, 'CORRELATION': 0.8385329806886566}, 'times': {'contamination': 0.001939535140991211, 'optimization': 6.223032236099243, 'imputation': 0.03267955780029297, 'log_imputation': -1.4857238287060839}}, '0.4': {'scores': {'RMSE': 0.5860009663014689, 'MAE': 0.44609007109014137, 'MI': 0.521244046221124, 'CORRELATION': 0.8153992558860045}, 'times': {'contamination': 0.010940790176391602, 'optimization': 6.223032236099243, 'imputation': 0.04111742973327637, 'log_imputation': -1.3859740410833805}}, '0.6': {'scores': {'RMSE': 0.5660313610410791, 'MAE': 0.4276393718227666, 'MI': 0.49353479991423727, 'CORRELATION': 0.8205221428625775}, 'times': {'contamination': 0.037363290786743164, 'optimization': 6.223032236099243, 'imputation': 0.03239703178405762, 'log_imputation': -1.4894947780296786}}, '0.8': {'scores': {'RMSE': 0.5961887193759151, 'MAE': 0.44923360559592973, 'MI': 0.4403528298201651, 'CORRELATION': 0.7923498783483066}, 'times': {'contamination': 0.13292860984802246, 'optimization': 6.223032236099243, 'imputation': 0.027922630310058594, 'log_imputation': -1.5540436736083756}}}}, 'dynammo': {'bayesian': {'0.05': {'scores': {'RMSE': 0.3403862066559318, 'MAE': 0.27356711160395475, 'MI': 1.5630422297119746, 'CORRELATION': 0.9674522356599553}, 'times': {'contamination': 0.0004918575286865234, 'optimization': 6.223032236099243, 'imputation': 0.6740424633026123, 'log_imputation': -0.1713127429348511}}, '0.1': {'scores': {'RMSE': 0.2666362985155662, 'MAE': 0.20418306046012286, 'MI': 1.1228031679070642, 'CORRELATION': 0.9510156008329083}, 'times': {'contamination': 0.0017666816711425781, 'optimization': 6.223032236099243, 'imputation': 0.551837682723999, 'log_imputation': -0.25818864666161717}}, '0.2': {'scores': {'RMSE': 0.29792570444078387, 'MAE': 0.21809646000116187, 'MI': 1.0117218812940276, 'CORRELATION': 0.9500921814409687}, 'times': {'contamination': 0.006150722503662109, 'optimization': 6.223032236099243, 'imputation': 2.747163772583008, 'log_imputation': 0.43888455072342525}}, '0.4': {'scores': {'RMSE': 0.348178909467498, 'MAE': 0.2655487041307776, 'MI': 0.9113779649332435, 'CORRELATION': 0.9415594392146491}, 'times': {'contamination': 0.02126026153564453, 'optimization': 6.223032236099243, 'imputation': 0.6828112602233887, 'log_imputation': -0.16569932555882722}}, '0.6': {'scores': {'RMSE': 0.4107774467667331, 'MAE': 0.3089190743400509, 'MI': 0.7388842161538886, 'CORRELATION': 0.9154131078751144}, 'times': {'contamination': 0.07302045822143555, 'optimization': 6.223032236099243, 'imputation': 1.5603094100952148, 'log_imputation': 0.1932107276959959}}, '0.8': {'scores': {'RMSE': 0.588290813346544, 'MAE': 0.4478690277877586, 'MI': 0.5109597106195052, 'CORRELATION': 0.8261083241361511}, 'times': {'contamination': 0.17532873153686523, 'optimization': 6.223032236099243, 'imputation': 0.6480617523193359, 'log_imputation': -0.18838360923165065}}}}, 'rosl': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5073073869101412, 'MAE': 0.4314923171329726, 'MI': 1.2822025415412734, 'CORRELATION': 0.8965671001416712}, 'times': {'contamination': 0.0009927749633789062, 'optimization': 6.223032236099243, 'imputation': 0.7367503643035889, 'log_imputation': -0.13267964073083768}}, '0.1': {'scores': {'RMSE': 0.5299186106839902, 'MAE': 0.3959016859288709, 'MI': 0.673974184554775, 'CORRELATION': 0.7905381854476283}, 'times': {'contamination': 0.001737833023071289, 'optimization': 6.223032236099243, 'imputation': 6.792823314666748, 'log_imputation': 0.8320503184824983}}, '0.2': {'scores': {'RMSE': 0.8048550260145149, 'MAE': 0.5360165060720303, 'MI': 0.4338193486854973, 'CORRELATION': 0.6201039356499416}, 'times': {'contamination': 0.004045724868774414, 'optimization': 6.223032236099243, 'imputation': 12.475021839141846, 'log_imputation': 1.0960413145848455}}, '0.4': {'scores': {'RMSE': 0.7572556918813225, 'MAE': 0.5529450768202853, 'MI': 0.36368683759488646, 'CORRELATION': 0.667544887668649}, 'times': {'contamination': 0.02777552604675293, 'optimization': 6.223032236099243, 'imputation': 6.48235011100769, 'log_imputation': 0.8117324835262565}}, '0.6': {'scores': {'RMSE': 0.780034070433024, 'MAE': 0.5904019383572706, 'MI': 0.24559864369576676, 'CORRELATION': 0.6184115402101897}, 'times': {'contamination': 0.09498357772827148, 'optimization': 6.223032236099243, 'imputation': 8.090100526809692, 'log_imputation': 0.9079539181471901}}, '0.8': {'scores': {'RMSE': 0.8963275025421664, 'MAE': 0.6990966709455917, 'MI': 0.09427622309511863, 'CORRELATION': 0.39504699696789775}, 'times': {'contamination': 0.19866085052490234, 'optimization': 6.223032236099243, 'imputation': 10.166579961776733, 'log_imputation': 1.007174880796059}}}}, 'soft_imp': {'bayesian': {'0.05': {'scores': {'RMSE': 1.107394798606378, 'MAE': 0.9036474830477748, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0010476112365722656, 'optimization': 6.223032236099243, 'imputation': 0.000339508056640625, 'log_imputation': -3.469149915306749}}, '0.1': {'scores': {'RMSE': 0.8569349076796438, 'MAE': 0.6416542359734557, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0017724037170410156, 'optimization': 6.223032236099243, 'imputation': 0.0002703666687011719, 'log_imputation': -3.5680468500506985}}, '0.2': {'scores': {'RMSE': 0.9609255264919324, 'MAE': 0.756013835497571, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00443577766418457, 'optimization': 6.223032236099243, 'imputation': 0.00031757354736328125, 'log_imputation': -3.498155679773304}}, '0.4': {'scores': {'RMSE': 1.0184989120725458, 'MAE': 0.8150966718352457, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.021195650100708008, 'optimization': 6.223032236099243, 'imputation': 0.0003352165222167969, 'log_imputation': -3.474674583923781}}, '0.6': {'scores': {'RMSE': 0.9997401940199045, 'MAE': 0.7985721718600829, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.08087277412414551, 'optimization': 6.223032236099243, 'imputation': 0.00035953521728515625, 'log_imputation': -3.444258563073831}}, '0.8': {'scores': {'RMSE': 0.9895691678332014, 'MAE': 0.7901674118013952, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.11553239822387695, 'optimization': 6.223032236099243, 'imputation': 0.00039649009704589844, 'log_imputation': -3.401767655388067}}}}, 'spirit': {'bayesian': {'0.05': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0009157657623291016, 'optimization': 6.223032236099243, 'imputation': 0.311901330947876, 'log_imputation': -0.5059827720139849}}, '0.1': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0008780956268310547, 'optimization': 6.223032236099243, 'imputation': 0.13858485221862793, 'log_imputation': -0.8582842369491839}}, '0.2': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.004143476486206055, 'optimization': 6.223032236099243, 'imputation': 0.12722134590148926, 'log_imputation': -0.8954400142421299}}, '0.4': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.011161565780639648, 'optimization': 6.223032236099243, 'imputation': 0.07907509803771973, 'log_imputation': -1.101960260971338}}, '0.6': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.04014873504638672, 'optimization': 6.223032236099243, 'imputation': 0.1584458351135254, 'log_imputation': -0.8001191721315302}}, '0.8': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.13056540489196777, 'optimization': 6.223032236099243, 'imputation': 0.08906126022338867, 'log_imputation': -1.0503111638624265}}}}, 'svt': {'bayesian': {'0.05': {'scores': {'RMSE': 0.19864890761921616, 'MAE': 0.15820305753043246, 'MI': 1.61637247989605, 'CORRELATION': 0.991804054758631}, 'times': {'contamination': 0.0007846355438232422, 'optimization': 6.223032236099243, 'imputation': 123.03512835502625, 'log_imputation': 2.090029126663987}}, '0.1': {'scores': {'RMSE': 0.1609449182837371, 'MAE': 0.11911901451723497, 'MI': 1.3378844729887542, 'CORRELATION': 0.9837939832928067}, 'times': {'contamination': 0.0016703605651855469, 'optimization': 6.223032236099243, 'imputation': 134.92491221427917, 'log_imputation': 2.1300921441738527}}, '0.2': {'scores': {'RMSE': 0.19189374525171293, 'MAE': 0.14161148602340873, 'MI': 1.2684251862810416, 'CORRELATION': 0.9804644957618451}, 'times': {'contamination': 0.0033714771270751953, 'optimization': 6.223032236099243, 'imputation': 136.71379470825195, 'log_imputation': 2.135812338001711}}, '0.4': {'scores': {'RMSE': 0.27363604739090247, 'MAE': 0.1960956220395044, 'MI': 1.0585563625749632, 'CORRELATION': 0.9665752998497383}, 'times': {'contamination': 0.022769451141357422, 'optimization': 6.223032236099243, 'imputation': 108.05165433883667, 'log_imputation': 2.0336314205920303}}, '0.6': {'scores': {'RMSE': 0.31632367551173785, 'MAE': 0.23243582154806275, 'MI': 0.8884616363906483, 'CORRELATION': 0.9518617420601576}, 'times': {'contamination': 0.07416486740112305, 'optimization': 6.223032236099243, 'imputation': 72.15566968917847, 'log_imputation': 1.8582704618048784}}, '0.8': {'scores': {'RMSE': 0.4342039820951686, 'MAE': 0.3270390569892163, 'MI': 0.7379348316124412, 'CORRELATION': 0.9146324058710877}, 'times': {'contamination': 0.16185379028320312, 'optimization': 6.223032236099243, 'imputation': 66.22069120407104, 'log_imputation': 1.8209937095562982}}}}, 'tkcm': {'bayesian': {'0.05': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0010685920715332031, 'optimization': 6.223032236099243, 'imputation': 0.2637288570404053, 'log_imputation': -0.5788423473861615}}, '0.1': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0009951591491699219, 'optimization': 6.223032236099243, 'imputation': 0.09778523445129395, 'log_imputation': -1.0097267186321455}}, '0.2': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0016584396362304688, 'optimization': 6.223032236099243, 'imputation': 0.14792680740356445, 'log_imputation': -0.8299531157092283}}, '0.4': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.06688308715820312, 'optimization': 6.223032236099243, 'imputation': 0.45121264457702637, 'log_imputation': -0.34561873838401685}}, '0.6': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.057092905044555664, 'optimization': 6.223032236099243, 'imputation': 0.3808269500732422, 'log_imputation': -0.41927232537698866}}, '0.8': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 1.0454187393188477, 'optimization': 6.223032236099243, 'imputation': 0.19805121421813965, 'log_imputation': -0.7032224906662957}}}}}}</t>
+    <t>{'mcar': {'cdrec': {'bayesian': {'0.05': {'scores': {'RMSE': 0.27605346336535824, 'MAE': 0.20172179379755226, 'MI': 1.6287285825717355, 'CORRELATION': 0.9838005973658245}, 'times': {'contamination': 0.00032258033752441406, 'optimization': 6.477632284164429, 'imputation': 1.3992314338684082, 'log_imputation': 0.14588955304741516}}, '0.1': {'scores': {'RMSE': 0.23232694306396792, 'MAE': 0.17310574767639833, 'MI': 1.1951438022350207, 'CORRELATION': 0.9640385877101987}, 'times': {'contamination': 0.0036585330963134766, 'optimization': 6.477632284164429, 'imputation': 1.4839262962341309, 'log_imputation': 0.17141233090681185}}, '0.2': {'scores': {'RMSE': 0.21804885816582129, 'MAE': 0.16264927399368448, 'MI': 1.184724280002774, 'CORRELATION': 0.9737339134318109}, 'times': {'contamination': 0.005358695983886719, 'optimization': 6.477632284164429, 'imputation': 3.8943920135498047, 'log_imputation': 0.5904396659186012}}, '0.4': {'scores': {'RMSE': 0.2848440560052875, 'MAE': 0.1955094245129383, 'MI': 1.0150919512842373, 'CORRELATION': 0.9596099121939262}, 'times': {'contamination': 0.02654576301574707, 'optimization': 6.477632284164429, 'imputation': 9.653903007507324, 'log_imputation': 0.9847029311601168}}, '0.6': {'scores': {'RMSE': 0.3411304383415171, 'MAE': 0.23465960462790825, 'MI': 0.8713081877855033, 'CORRELATION': 0.9402245657713347}, 'times': {'contamination': 0.06874918937683105, 'optimization': 6.477632284164429, 'imputation': 27.957423448562622, 'log_imputation': 1.4464971444115333}}, '0.8': {'scores': {'RMSE': 0.5679458730957042, 'MAE': 0.37489302674430003, 'MI': 0.5716189408134524, 'CORRELATION': 0.8410496841608827}, 'times': {'contamination': 0.10736489295959473, 'optimization': 6.477632284164429, 'imputation': 135.0705304145813, 'log_imputation': 2.130560605318027}}}}, 'iter_svd': {'bayesian': {'0.05': {'scores': {'RMSE': 1.107394798606378, 'MAE': 0.9036474830477748, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0027649402618408203, 'optimization': 6.477632284164429, 'imputation': 0.0004093647003173828, 'log_imputation': -3.38788960944667}}, '0.1': {'scores': {'RMSE': 0.8569349076796438, 'MAE': 0.6416542359734557, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0032134056091308594, 'optimization': 6.477632284164429, 'imputation': 0.0003764629364013672, 'log_imputation': -3.4242777745992923}}, '0.2': {'scores': {'RMSE': 0.9609255264919324, 'MAE': 0.756013835497571, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.010840654373168945, 'optimization': 6.477632284164429, 'imputation': 0.00033211708068847656, 'log_imputation': -3.478708788183623}}, '0.4': {'scores': {'RMSE': 1.0184989120725458, 'MAE': 0.8150966718352457, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.01994633674621582, 'optimization': 6.477632284164429, 'imputation': 0.00037980079650878906, 'log_imputation': -3.4204441288064547}}, '0.6': {'scores': {'RMSE': 0.9997401940199045, 'MAE': 0.7985721718600829, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.018753528594970703, 'optimization': 6.477632284164429, 'imputation': 0.0002052783966064453, 'log_imputation': -3.6876567531539317}}, '0.8': {'scores': {'RMSE': 0.9895691678332014, 'MAE': 0.7901674118013952, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.052106380462646484, 'optimization': 6.477632284164429, 'imputation': 0.00021505355834960938, 'log_imputation': -3.6674533670656446}}}}, 'grouse': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5148496955923699, 'MAE': 0.415876537807372, 'MI': 1.3401665927292032, 'CORRELATION': 0.9150576799948262}, 'times': {'contamination': 0.0002617835998535156, 'optimization': 6.477632284164429, 'imputation': 0.039891719818115234, 'log_imputation': -1.3991172399143597}}, '0.1': {'scores': {'RMSE': 0.5514172365414519, 'MAE': 0.4246206846745574, 'MI': 0.605160166686089, 'CORRELATION': 0.7646002717223995}, 'times': {'contamination': 0.00043511390686035156, 'optimization': 6.477632284164429, 'imputation': 0.01768970489501953, 'log_imputation': -1.752279412061086}}, '0.2': {'scores': {'RMSE': 0.5224946657403522, 'MAE': 0.4039231091274249, 'MI': 0.6011853028388328, 'CORRELATION': 0.8385329806886566}, 'times': {'contamination': 0.0010046958923339844, 'optimization': 6.477632284164429, 'imputation': 0.015034198760986328, 'log_imputation': -1.8229197124224386}}, '0.4': {'scores': {'RMSE': 0.5860009663014689, 'MAE': 0.44609007109014137, 'MI': 0.521244046221124, 'CORRELATION': 0.8153992558860045}, 'times': {'contamination': 0.005591154098510742, 'optimization': 6.477632284164429, 'imputation': 0.012361288070678711, 'log_imputation': -1.9079362725448037}}, '0.6': {'scores': {'RMSE': 0.5660313610410791, 'MAE': 0.4276393718227666, 'MI': 0.49353479991423727, 'CORRELATION': 0.8205221428625775}, 'times': {'contamination': 0.01544189453125, 'optimization': 6.477632284164429, 'imputation': 0.011534452438354492, 'log_imputation': -1.9380030174103804}}, '0.8': {'scores': {'RMSE': 0.5961887193759151, 'MAE': 0.44923360559592973, 'MI': 0.4403528298201651, 'CORRELATION': 0.7923498783483066}, 'times': {'contamination': 0.04788470268249512, 'optimization': 6.477632284164429, 'imputation': 0.012183904647827148, 'log_imputation': -1.9142135084806604}}}}, 'dynammo': {'bayesian': {'0.05': {'scores': {'RMSE': 0.3403862066559318, 'MAE': 0.27356711160395475, 'MI': 1.5630422297119746, 'CORRELATION': 0.9674522356599553}, 'times': {'contamination': 0.0002391338348388672, 'optimization': 6.477632284164429, 'imputation': 9.744339942932129, 'log_imputation': 0.9887524264345655}}, '0.1': {'scores': {'RMSE': 0.2666362985155662, 'MAE': 0.20418306046012286, 'MI': 1.1228031679070642, 'CORRELATION': 0.9510156008329083}, 'times': {'contamination': 0.007864236831665039, 'optimization': 6.477632284164429, 'imputation': 11.703598737716675, 'log_imputation': 1.0683194234228937}}, '0.2': {'scores': {'RMSE': 0.29792570444078387, 'MAE': 0.21809646000116187, 'MI': 1.0117218812940276, 'CORRELATION': 0.9500921814409687}, 'times': {'contamination': 0.004745960235595703, 'optimization': 6.477632284164429, 'imputation': 8.310850620269775, 'log_imputation': 0.9196454763453091}}, '0.4': {'scores': {'RMSE': 0.348178909467498, 'MAE': 0.2655487041307776, 'MI': 0.9113779649332435, 'CORRELATION': 0.9415594392146491}, 'times': {'contamination': 0.026737451553344727, 'optimization': 6.477632284164429, 'imputation': 4.934169292449951, 'log_imputation': 0.693214046149975}}, '0.6': {'scores': {'RMSE': 0.4107774467667331, 'MAE': 0.3089190743400509, 'MI': 0.7388842161538886, 'CORRELATION': 0.9154131078751144}, 'times': {'contamination': 0.07286357879638672, 'optimization': 6.477632284164429, 'imputation': 5.074278831481934, 'log_imputation': 0.7053743280112226}}, '0.8': {'scores': {'RMSE': 0.588290813346544, 'MAE': 0.4478690277877586, 'MI': 0.5109597106195052, 'CORRELATION': 0.8261083241361511}, 'times': {'contamination': 0.11254549026489258, 'optimization': 6.477632284164429, 'imputation': 10.175788402557373, 'log_imputation': 1.007568067589209}}}}, 'rosl': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5073073869101417, 'MAE': 0.4314923171329729, 'MI': 1.2822025415412734, 'CORRELATION': 0.8965671001416712}, 'times': {'contamination': 0.005505800247192383, 'optimization': 6.477632284164429, 'imputation': 18.640565872192383, 'log_imputation': 1.2704590921081116}}, '0.1': {'scores': {'RMSE': 0.5299186106839897, 'MAE': 0.39590168592887065, 'MI': 0.673974184554775, 'CORRELATION': 0.7905381854476284}, 'times': {'contamination': 0.006900787353515625, 'optimization': 6.477632284164429, 'imputation': 55.519734144210815, 'log_imputation': 1.7444473778362317}}, '0.2': {'scores': {'RMSE': 0.8048550260145149, 'MAE': 0.5360165060720301, 'MI': 0.4338193486854973, 'CORRELATION': 0.620103935649942}, 'times': {'contamination': 0.003606557846069336, 'optimization': 6.477632284164429, 'imputation': 53.56450867652893, 'log_imputation': 1.7288771256761506}}, '0.4': {'scores': {'RMSE': 0.7572556918813218, 'MAE': 0.552945076820285, 'MI': 0.36368683759488646, 'CORRELATION': 0.6675448876686496}, 'times': {'contamination': 0.013316869735717773, 'optimization': 6.477632284164429, 'imputation': 54.6838264465332, 'log_imputation': 1.7378588962848072}}, '0.6': {'scores': {'RMSE': 0.7800340704330233, 'MAE': 0.5904019383572702, 'MI': 0.24559864369576676, 'CORRELATION': 0.6184115402101905}, 'times': {'contamination': 0.028061866760253906, 'optimization': 6.477632284164429, 'imputation': 51.93647527694702, 'log_imputation': 1.7154724724454875}}, '0.8': {'scores': {'RMSE': 0.8963275025421662, 'MAE': 0.6990966709455915, 'MI': 0.09427622309511863, 'CORRELATION': 0.3950469969678982}, 'times': {'contamination': 0.08399319648742676, 'optimization': 6.477632284164429, 'imputation': 50.91719388961792, 'log_imputation': 1.70686446112782}}}}, 'soft_imp': {'bayesian': {'0.05': {'scores': {'RMSE': 1.107394798606378, 'MAE': 0.9036474830477748, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.001573324203491211, 'optimization': 6.477632284164429, 'imputation': 0.0002009868621826172, 'log_imputation': -3.696832329982844}}, '0.1': {'scores': {'RMSE': 0.8569349076796438, 'MAE': 0.6416542359734557, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.001773834228515625, 'optimization': 6.477632284164429, 'imputation': 0.000164031982421875, 'log_imputation': -3.785071466372075}}, '0.2': {'scores': {'RMSE': 0.9609255264919324, 'MAE': 0.756013835497571, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0038383007049560547, 'optimization': 6.477632284164429, 'imputation': 0.0002028942108154297, 'log_imputation': -3.6927303445229986}}, '0.4': {'scores': {'RMSE': 1.0184989120725458, 'MAE': 0.8150966718352457, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.010627031326293945, 'optimization': 6.477632284164429, 'imputation': 0.00023245811462402344, 'log_imputation': -3.6336552889090497}}, '0.6': {'scores': {'RMSE': 0.9997401940199045, 'MAE': 0.7985721718600829, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.04246950149536133, 'optimization': 6.477632284164429, 'imputation': 0.00029659271240234375, 'log_imputation': -3.5278395242527862}}, '0.8': {'scores': {'RMSE': 0.9895691678332014, 'MAE': 0.7901674118013952, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.06438636779785156, 'optimization': 6.477632284164429, 'imputation': 0.00028967857360839844, 'log_imputation': -3.5380836266732554}}}}, 'spirit': {'bayesian': {'0.05': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00028777122497558594, 'optimization': 6.477632284164429, 'imputation': 0.04762911796569824, 'log_imputation': -1.3221274610283427}}, '0.1': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0007073879241943359, 'optimization': 6.477632284164429, 'imputation': 0.034802913665771484, 'log_imputation': -1.4583843958236309}}, '0.2': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0012459754943847656, 'optimization': 6.477632284164429, 'imputation': 0.03215479850769043, 'log_imputation': -1.4927542075015947}}, '0.4': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.004374265670776367, 'optimization': 6.477632284164429, 'imputation': 0.03075265884399414, 'log_imputation': -1.5121173296005828}}, '0.6': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.01365804672241211, 'optimization': 6.477632284164429, 'imputation': 0.029462814331054688, 'log_imputation': -1.5307257710687456}}, '0.8': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.053224802017211914, 'optimization': 6.477632284164429, 'imputation': 0.03213071823120117, 'log_imputation': -1.4930795663762413}}}}, 'svt': {'bayesian': {'0.05': {'scores': {'RMSE': 0.19864890761921392, 'MAE': 0.15820305753043434, 'MI': 1.61637247989605, 'CORRELATION': 0.9918040547586304}, 'times': {'contamination': 0.0003256797790527344, 'optimization': 6.477632284164429, 'imputation': 82.85739278793335, 'log_imputation': 1.9183312635552257}}, '0.1': {'scores': {'RMSE': 0.16094491828373556, 'MAE': 0.11911901451724377, 'MI': 1.3378844729887542, 'CORRELATION': 0.9837939832928086}, 'times': {'contamination': 0.004145622253417969, 'optimization': 6.477632284164429, 'imputation': 88.29764556884766, 'log_imputation': 1.9459491233953499}}, '0.2': {'scores': {'RMSE': 0.1918937452517292, 'MAE': 0.14161148602341808, 'MI': 1.2684251862810416, 'CORRELATION': 0.9804644957618428}, 'times': {'contamination': 0.016449928283691406, 'optimization': 6.477632284164429, 'imputation': 85.92550134658813, 'log_imputation': 1.9341220747798367}}, '0.4': {'scores': {'RMSE': 0.2736360473909011, 'MAE': 0.19609562203950157, 'MI': 1.0585563625749632, 'CORRELATION': 0.9665752998497372}, 'times': {'contamination': 0.01042795181274414, 'optimization': 6.477632284164429, 'imputation': 68.8833863735199, 'log_imputation': 1.8381144893048122}}, '0.6': {'scores': {'RMSE': 0.3163236755117419, 'MAE': 0.23243582154806755, 'MI': 0.8884616363906483, 'CORRELATION': 0.9518617420601588}, 'times': {'contamination': 0.06060647964477539, 'optimization': 6.477632284164429, 'imputation': 46.41817092895508, 'log_imputation': 1.666688023428988}}, '0.8': {'scores': {'RMSE': 0.43420398209517674, 'MAE': 0.327039056989223, 'MI': 0.7379348316124412, 'CORRELATION': 0.9146324058710882}, 'times': {'contamination': 0.10345578193664551, 'optimization': 6.477632284164429, 'imputation': 36.39370512962341, 'log_imputation': 1.561026272003872}}}}, 'tkcm': {'bayesian': {'0.05': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0027208328247070312, 'optimization': 6.477632284164429, 'imputation': 0.03332209587097168, 'log_imputation': -1.4772676904413662}}, '0.1': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0007138252258300781, 'optimization': 6.477632284164429, 'imputation': 0.008727073669433594, 'log_imputation': -2.0591313579288375}}, '0.2': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0009438991546630859, 'optimization': 6.477632284164429, 'imputation': 0.008991479873657227, 'log_imputation': -2.0461688234980855}}, '0.4': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.004921674728393555, 'optimization': 6.477632284164429, 'imputation': 0.00987386703491211, 'log_imputation': -2.0055127254447003}}, '0.6': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.015380859375, 'optimization': 6.477632284164429, 'imputation': 0.012686014175415039, 'log_imputation': -1.89667480765548}}, '0.8': {'scores': {'RMSE': 100.0, 'MAE': 100, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.04205679893493652, 'optimization': 6.477632284164429, 'imputation': 0.02692437171936035, 'log_imputation': -1.5698544221803408}}}}}}</t>
   </si>
   <si>
     <t>RMSE: Root Mean Square Error - Measures the average magnitude of error.</t>

</xml_diff>